<commit_message>
BUG FIX 1.)BTP SINGLE EXPORT 2.)DSR FROM VALIDATION
</commit_message>
<xml_diff>
--- a/src/main/resources/empty-templates/SELECTED_BTP_DETAIL_XLS_TEMPLATE.xlsx
+++ b/src/main/resources/empty-templates/SELECTED_BTP_DETAIL_XLS_TEMPLATE.xlsx
@@ -4,26 +4,18 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="120" windowWidth="19020" windowHeight="8325"/>
+    <workbookView xWindow="0" yWindow="2445" windowWidth="23955" windowHeight="8685"/>
   </bookViews>
   <sheets>
     <sheet name="BTPReport" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="38">
-  <si>
-    <t>Suresh Kannan</t>
-  </si>
-  <si>
-    <t>Prem Anandakrishnan</t>
-  </si>
-  <si>
-    <t>Saranya Rajendran</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="35">
   <si>
     <t>S.No</t>
   </si>
@@ -647,45 +639,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="11" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="16" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="9" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="20" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="10" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="11" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="15" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="16" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="21" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="26" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="22" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="25" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -698,11 +651,14 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="14" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="23" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="24" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="29" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -722,14 +678,50 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="28" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="23" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="24" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="11" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="16" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="9" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="20" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="10" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="11" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="15" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="16" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="21" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="26" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="22" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="25" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -1038,7 +1030,7 @@
   <dimension ref="A1:I22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H22" sqref="H22:I22"/>
+      <selection activeCell="B10" sqref="B10:C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1053,147 +1045,141 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A1" s="47" t="s">
-        <v>24</v>
-      </c>
-      <c r="B1" s="48"/>
-      <c r="C1" s="48"/>
-      <c r="D1" s="48"/>
-      <c r="E1" s="48"/>
-      <c r="F1" s="48"/>
-      <c r="G1" s="48"/>
-      <c r="H1" s="48"/>
-      <c r="I1" s="49"/>
+      <c r="A1" s="26" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" s="27"/>
+      <c r="C1" s="27"/>
+      <c r="D1" s="27"/>
+      <c r="E1" s="27"/>
+      <c r="F1" s="27"/>
+      <c r="G1" s="27"/>
+      <c r="H1" s="27"/>
+      <c r="I1" s="28"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="10" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B2" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="C2" s="22" t="s">
-        <v>18</v>
-      </c>
-      <c r="D2" s="41" t="s">
-        <v>0</v>
-      </c>
-      <c r="E2" s="42"/>
-      <c r="F2" s="43" t="s">
-        <v>1</v>
-      </c>
-      <c r="G2" s="44"/>
+        <v>20</v>
+      </c>
+      <c r="C2" s="37" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" s="29"/>
+      <c r="E2" s="30"/>
+      <c r="F2" s="31"/>
+      <c r="G2" s="32"/>
       <c r="H2" s="11"/>
       <c r="I2" s="19"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="13" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="C3" s="23"/>
-      <c r="D3" s="45" t="s">
-        <v>2</v>
-      </c>
-      <c r="E3" s="46"/>
-      <c r="F3" s="37"/>
-      <c r="G3" s="38"/>
+      <c r="C3" s="38"/>
+      <c r="D3" s="33"/>
+      <c r="E3" s="34"/>
+      <c r="F3" s="24"/>
+      <c r="G3" s="25"/>
       <c r="H3" s="11"/>
       <c r="I3" s="17"/>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B4" s="14">
         <v>41850</v>
       </c>
-      <c r="C4" s="23"/>
-      <c r="D4" s="37"/>
-      <c r="E4" s="38"/>
-      <c r="F4" s="37"/>
-      <c r="G4" s="38"/>
+      <c r="C4" s="38"/>
+      <c r="D4" s="24"/>
+      <c r="E4" s="25"/>
+      <c r="F4" s="24"/>
+      <c r="G4" s="25"/>
       <c r="H4" s="11"/>
       <c r="I4" s="17"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B5" s="15">
         <v>41850</v>
       </c>
-      <c r="C5" s="23"/>
-      <c r="D5" s="37"/>
-      <c r="E5" s="38"/>
-      <c r="F5" s="37"/>
-      <c r="G5" s="38"/>
+      <c r="C5" s="38"/>
+      <c r="D5" s="24"/>
+      <c r="E5" s="25"/>
+      <c r="F5" s="24"/>
+      <c r="G5" s="25"/>
       <c r="H5" s="12"/>
       <c r="I5" s="18"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B6" s="16">
         <v>42636</v>
       </c>
-      <c r="C6" s="24"/>
-      <c r="D6" s="37"/>
-      <c r="E6" s="38"/>
-      <c r="F6" s="37"/>
-      <c r="G6" s="38"/>
+      <c r="C6" s="39"/>
+      <c r="D6" s="24"/>
+      <c r="E6" s="25"/>
+      <c r="F6" s="24"/>
+      <c r="G6" s="25"/>
       <c r="H6" s="12"/>
       <c r="I6" s="18"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="25" t="s">
+      <c r="A7" s="40" t="s">
+        <v>0</v>
+      </c>
+      <c r="B7" s="42" t="s">
+        <v>1</v>
+      </c>
+      <c r="C7" s="43"/>
+      <c r="D7" s="46" t="s">
+        <v>2</v>
+      </c>
+      <c r="E7" s="35" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="27" t="s">
+      <c r="F7" s="36"/>
+      <c r="G7" s="48" t="s">
+        <v>6</v>
+      </c>
+      <c r="H7" s="42" t="s">
+        <v>7</v>
+      </c>
+      <c r="I7" s="43"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="41"/>
+      <c r="B8" s="44"/>
+      <c r="C8" s="45"/>
+      <c r="D8" s="47"/>
+      <c r="E8" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="28"/>
-      <c r="D7" s="31" t="s">
+      <c r="F8" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="E7" s="39" t="s">
-        <v>6</v>
-      </c>
-      <c r="F7" s="40"/>
-      <c r="G7" s="33" t="s">
-        <v>9</v>
-      </c>
-      <c r="H7" s="27" t="s">
-        <v>10</v>
-      </c>
-      <c r="I7" s="28"/>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="26"/>
-      <c r="B8" s="29"/>
-      <c r="C8" s="30"/>
-      <c r="D8" s="32"/>
-      <c r="E8" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="F8" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="G8" s="34"/>
-      <c r="H8" s="29"/>
-      <c r="I8" s="30"/>
+      <c r="G8" s="49"/>
+      <c r="H8" s="44"/>
+      <c r="I8" s="45"/>
     </row>
     <row r="9" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="8">
         <v>1</v>
       </c>
-      <c r="B9" s="35" t="s">
-        <v>11</v>
-      </c>
-      <c r="C9" s="36"/>
+      <c r="B9" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9" s="23"/>
       <c r="D9" s="1">
         <v>56</v>
       </c>
@@ -1204,10 +1190,10 @@
         <v>12</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="H9" s="21" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="I9" s="21"/>
     </row>
@@ -1216,7 +1202,7 @@
         <v>2</v>
       </c>
       <c r="B10" s="20" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C10" s="20"/>
       <c r="D10" s="1">
@@ -1229,10 +1215,10 @@
         <v>12</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="H10" s="21" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="I10" s="21"/>
     </row>
@@ -1241,7 +1227,7 @@
         <v>3</v>
       </c>
       <c r="B11" s="20" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C11" s="20"/>
       <c r="D11" s="1">
@@ -1254,10 +1240,10 @@
         <v>12</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="H11" s="21" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="I11" s="21"/>
     </row>
@@ -1266,7 +1252,7 @@
         <v>4</v>
       </c>
       <c r="B12" s="20" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C12" s="20"/>
       <c r="D12" s="1">
@@ -1279,10 +1265,10 @@
         <v>12</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="H12" s="21" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="I12" s="21"/>
     </row>
@@ -1291,7 +1277,7 @@
         <v>5</v>
       </c>
       <c r="B13" s="20" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C13" s="20"/>
       <c r="D13" s="1">
@@ -1304,10 +1290,10 @@
         <v>12</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="H13" s="21" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="I13" s="21"/>
     </row>
@@ -1316,7 +1302,7 @@
         <v>6</v>
       </c>
       <c r="B14" s="20" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C14" s="20"/>
       <c r="D14" s="1">
@@ -1329,10 +1315,10 @@
         <v>12</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="H14" s="21" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="I14" s="21"/>
     </row>
@@ -1341,7 +1327,7 @@
         <v>7</v>
       </c>
       <c r="B15" s="20" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C15" s="20"/>
       <c r="D15" s="1">
@@ -1354,10 +1340,10 @@
         <v>12</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="H15" s="21" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="I15" s="21"/>
     </row>
@@ -1365,10 +1351,10 @@
       <c r="A16" s="8">
         <v>8</v>
       </c>
-      <c r="B16" s="35" t="s">
-        <v>11</v>
-      </c>
-      <c r="C16" s="36"/>
+      <c r="B16" s="22" t="s">
+        <v>8</v>
+      </c>
+      <c r="C16" s="23"/>
       <c r="D16" s="1">
         <v>56</v>
       </c>
@@ -1379,10 +1365,10 @@
         <v>12</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="H16" s="21" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="I16" s="21"/>
     </row>
@@ -1391,7 +1377,7 @@
         <v>9</v>
       </c>
       <c r="B17" s="20" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C17" s="20"/>
       <c r="D17" s="1">
@@ -1404,10 +1390,10 @@
         <v>12</v>
       </c>
       <c r="G17" s="2" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="H17" s="21" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="I17" s="21"/>
     </row>
@@ -1416,7 +1402,7 @@
         <v>10</v>
       </c>
       <c r="B18" s="20" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C18" s="20"/>
       <c r="D18" s="1">
@@ -1429,10 +1415,10 @@
         <v>12</v>
       </c>
       <c r="G18" s="2" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="H18" s="21" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="I18" s="21"/>
     </row>
@@ -1441,7 +1427,7 @@
         <v>11</v>
       </c>
       <c r="B19" s="20" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C19" s="20"/>
       <c r="D19" s="1">
@@ -1454,10 +1440,10 @@
         <v>12</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="H19" s="21" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="I19" s="21"/>
     </row>
@@ -1466,7 +1452,7 @@
         <v>12</v>
       </c>
       <c r="B20" s="20" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C20" s="20"/>
       <c r="D20" s="1">
@@ -1479,10 +1465,10 @@
         <v>12</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="H20" s="21" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="I20" s="21"/>
     </row>
@@ -1491,7 +1477,7 @@
         <v>13</v>
       </c>
       <c r="B21" s="20" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C21" s="20"/>
       <c r="D21" s="1">
@@ -1504,10 +1490,10 @@
         <v>12</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="H21" s="21" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="I21" s="21"/>
     </row>
@@ -1516,7 +1502,7 @@
         <v>14</v>
       </c>
       <c r="B22" s="20" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="C22" s="20"/>
       <c r="D22" s="1">
@@ -1529,45 +1515,15 @@
         <v>12</v>
       </c>
       <c r="G22" s="2" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="H22" s="21" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="I22" s="21"/>
     </row>
   </sheetData>
   <mergeCells count="46">
-    <mergeCell ref="B22:C22"/>
-    <mergeCell ref="H22:I22"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="H19:I19"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="H20:I20"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="H21:I21"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="H16:I16"/>
-    <mergeCell ref="B17:C17"/>
-    <mergeCell ref="H17:I17"/>
-    <mergeCell ref="B18:C18"/>
-    <mergeCell ref="H18:I18"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="F5:G5"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="F4:G4"/>
-    <mergeCell ref="A1:I1"/>
-    <mergeCell ref="D2:E2"/>
-    <mergeCell ref="F2:G2"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="F3:G3"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="H10:I10"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="H11:I11"/>
-    <mergeCell ref="D6:E6"/>
-    <mergeCell ref="F6:G6"/>
-    <mergeCell ref="E7:F7"/>
     <mergeCell ref="B15:C15"/>
     <mergeCell ref="H15:I15"/>
     <mergeCell ref="C2:C6"/>
@@ -1584,6 +1540,36 @@
     <mergeCell ref="H14:I14"/>
     <mergeCell ref="B9:C9"/>
     <mergeCell ref="H9:I9"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="H10:I10"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="H11:I11"/>
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="F6:G6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="F5:G5"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="A1:I1"/>
+    <mergeCell ref="D2:E2"/>
+    <mergeCell ref="F2:G2"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="H16:I16"/>
+    <mergeCell ref="B17:C17"/>
+    <mergeCell ref="H17:I17"/>
+    <mergeCell ref="B18:C18"/>
+    <mergeCell ref="H18:I18"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="H22:I22"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="H19:I19"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="H20:I20"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="H21:I21"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>